<commit_message>
polished print sizes, implemented storing to db
</commit_message>
<xml_diff>
--- a/EdAsStExample.xlsx
+++ b/EdAsStExample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Software\Trash\IntelliJ IDEA 2020.3.2\workspace\SLDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EF528DB-2B61-46E3-A64C-736881FBE606}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B6A429-F3DE-4335-94BF-AAE5076E4118}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1425" windowWidth="28800" windowHeight="11385" tabRatio="924" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="924" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Осінь 1-3" sheetId="28" r:id="rId1"/>
@@ -19,6 +19,10 @@
     <sheet name="Весна 4" sheetId="23" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Весна 1-3'!$A$1:$H$59</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'Весна 4'!$A$1:$H$60</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Осінь 1-3'!$A$1:$H$82</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Осінь 4'!$A$1:$H$49</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'Весна 1-3'!$5:$6</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="3">'Весна 4'!$5:$6</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Осінь 1-3'!$5:$6</definedName>
@@ -993,8 +997,8 @@
   </sheetPr>
   <dimension ref="A1:S137"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="D165" sqref="D165"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -2488,7 +2492,7 @@
     <mergeCell ref="H5:H6"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="73" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="76" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
@@ -2502,7 +2506,7 @@
   <dimension ref="A1:I58"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40:D40"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2974,7 +2978,7 @@
     <mergeCell ref="H5:H6"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="74" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="80" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
@@ -2988,7 +2992,7 @@
   <dimension ref="A1:S173"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -4842,7 +4846,7 @@
     <mergeCell ref="H5:H6"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="75" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="76" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
@@ -4855,8 +4859,8 @@
   </sheetPr>
   <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C92" sqref="C92"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -5360,7 +5364,7 @@
     <mergeCell ref="H5:H6"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="74" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="80" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>